<commit_message>
updated raw data removed old trend frekvens code
</commit_message>
<xml_diff>
--- a/output05_color_tables_from_Rcode_for_MST2017_2022samples/table10_App_C_2018_02_autumn_table_eDNA_evalu.xlsx
+++ b/output05_color_tables_from_Rcode_for_MST2017_2022samples/table10_App_C_2018_02_autumn_table_eDNA_evalu.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="75">
   <si>
     <t>genus_species_aar</t>
   </si>
@@ -210,9 +210,6 @@
   </si>
   <si>
     <t>'2/0/0/1'</t>
-  </si>
-  <si>
-    <t>'2/0/1/0'</t>
   </si>
   <si>
     <t>'1/0/0/0'</t>
@@ -677,7 +674,7 @@
         <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
         <v>59</v>
@@ -692,7 +689,7 @@
         <v>59</v>
       </c>
       <c r="K7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L7" t="s">
         <v>59</v>
@@ -931,7 +928,7 @@
         <v>59</v>
       </c>
       <c r="H11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I11" t="s">
         <v>61</v>
@@ -990,7 +987,7 @@
         <v>60</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" t="s">
         <v>60</v>
@@ -1020,7 +1017,7 @@
         <v>60</v>
       </c>
       <c r="Q12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R12" t="s">
         <v>60</v>
@@ -1079,16 +1076,16 @@
         <v>59</v>
       </c>
       <c r="P13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q13" t="s">
         <v>59</v>
       </c>
       <c r="R13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T13" t="s">
         <v>59</v>
@@ -1108,7 +1105,7 @@
         <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
         <v>59</v>
@@ -1368,40 +1365,40 @@
         <v>62</v>
       </c>
       <c r="I18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K18" t="s">
         <v>62</v>
       </c>
       <c r="L18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q18" t="s">
         <v>63</v>
       </c>
       <c r="R18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19">
@@ -1439,13 +1436,13 @@
         <v>59</v>
       </c>
       <c r="L19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M19" t="s">
         <v>59</v>
       </c>
       <c r="N19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O19" t="s">
         <v>59</v>
@@ -1460,10 +1457,10 @@
         <v>59</v>
       </c>
       <c r="S19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20">
@@ -1489,7 +1486,7 @@
         <v>59</v>
       </c>
       <c r="H20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I20" t="s">
         <v>59</v>

</xml_diff>